<commit_message>
update readme for worldview outputs
</commit_message>
<xml_diff>
--- a/inputs/lsib_extension/adm0_points.xlsx
+++ b/inputs/lsib_extension/adm0_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/computer/GitHub/fieldmaps/adm0-generator/inputs/lsib_extension/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DE1824-104D-404E-A8FC-B966A0928269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E72DA9-B0FC-C94B-BC02-CE7301BE589C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20560" yWindow="880" windowWidth="20560" windowHeight="25700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="adm0_points" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">adm0_points!$A$1:$AE$319</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">adm0_points!$A$1:$AF$319</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2885" uniqueCount="1352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="1353">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -4093,6 +4093,9 @@
   </si>
   <si>
     <t>wld_notes</t>
+  </si>
+  <si>
+    <t>wld_view</t>
   </si>
 </sst>
 </file>
@@ -4447,7 +4450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE325"/>
+  <dimension ref="A1:AF325"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -4479,10 +4482,11 @@
     <col min="28" max="28" width="25.5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="161.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="161.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>1022</v>
       </c>
@@ -4574,10 +4578,13 @@
         <v>1350</v>
       </c>
       <c r="AE1" t="s">
+        <v>1352</v>
+      </c>
+      <c r="AF1" t="s">
         <v>1351</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>760</v>
       </c>
@@ -4624,7 +4631,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>761</v>
       </c>
@@ -4662,7 +4669,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>762</v>
       </c>
@@ -4706,7 +4713,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>763</v>
       </c>
@@ -4753,7 +4760,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>1023</v>
       </c>
@@ -4794,7 +4801,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>764</v>
       </c>
@@ -4832,7 +4839,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>765</v>
       </c>
@@ -4870,7 +4877,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>766</v>
       </c>
@@ -4908,7 +4915,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>767</v>
       </c>
@@ -4952,7 +4959,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>768</v>
       </c>
@@ -4990,7 +4997,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>769</v>
       </c>
@@ -5031,7 +5038,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>770</v>
       </c>
@@ -5057,7 +5064,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>1240</v>
       </c>
@@ -5104,7 +5111,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>1241</v>
       </c>
@@ -5151,7 +5158,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>1242</v>
       </c>
@@ -7903,7 +7910,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>825</v>
       </c>
@@ -7947,7 +7954,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
         <v>826</v>
       </c>
@@ -7994,7 +8001,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>827</v>
       </c>
@@ -8032,7 +8039,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
         <v>828</v>
       </c>
@@ -8070,7 +8077,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>829</v>
       </c>
@@ -8108,7 +8115,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
         <v>830</v>
       </c>
@@ -8146,7 +8153,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
         <v>831</v>
       </c>
@@ -8190,7 +8197,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
         <v>832</v>
       </c>
@@ -8228,7 +8235,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
         <v>833</v>
       </c>
@@ -8266,7 +8273,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
         <v>834</v>
       </c>
@@ -8312,11 +8319,11 @@
       <c r="AB90" t="s">
         <v>1333</v>
       </c>
-      <c r="AE90" t="s">
+      <c r="AF90" t="s">
         <v>1230</v>
       </c>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
         <v>835</v>
       </c>
@@ -8354,7 +8361,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
         <v>836</v>
       </c>
@@ -8395,7 +8402,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
         <v>837</v>
       </c>
@@ -8433,7 +8440,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
         <v>838</v>
       </c>
@@ -8477,7 +8484,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
         <v>839</v>
       </c>
@@ -8515,7 +8522,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="96" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
         <v>1031</v>
       </c>
@@ -9269,7 +9276,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="113" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
         <v>854</v>
       </c>
@@ -9313,7 +9320,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="114" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
         <v>855</v>
       </c>
@@ -9357,7 +9364,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="115" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
         <v>856</v>
       </c>
@@ -9398,7 +9405,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="116" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
         <v>857</v>
       </c>
@@ -9442,7 +9449,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="117" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
         <v>858</v>
       </c>
@@ -9480,7 +9487,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="118" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
         <v>859</v>
       </c>
@@ -9524,7 +9531,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="119" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
         <v>860</v>
       </c>
@@ -9562,7 +9569,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="120" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
         <v>861</v>
       </c>
@@ -9600,7 +9607,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="121" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
         <v>862</v>
       </c>
@@ -9641,7 +9648,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="122" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
         <v>863</v>
       </c>
@@ -9679,7 +9686,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="123" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
         <v>864</v>
       </c>
@@ -9725,11 +9732,11 @@
       <c r="AB123" t="s">
         <v>1328</v>
       </c>
-      <c r="AE123" t="s">
+      <c r="AF123" t="s">
         <v>1229</v>
       </c>
     </row>
-    <row r="124" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
         <v>865</v>
       </c>
@@ -9767,7 +9774,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="125" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
         <v>866</v>
       </c>
@@ -9805,7 +9812,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="126" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
         <v>867</v>
       </c>
@@ -9843,7 +9850,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="127" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
         <v>868</v>
       </c>
@@ -9881,7 +9888,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="128" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
         <v>869</v>
       </c>
@@ -13166,7 +13173,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="209" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A209" t="s">
         <v>946</v>
       </c>
@@ -13204,7 +13211,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="210" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A210" t="s">
         <v>947</v>
       </c>
@@ -13242,7 +13249,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="211" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A211" t="s">
         <v>948</v>
       </c>
@@ -13286,7 +13293,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="212" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A212" t="s">
         <v>949</v>
       </c>
@@ -13324,7 +13331,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="213" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A213" t="s">
         <v>950</v>
       </c>
@@ -13361,11 +13368,11 @@
       <c r="AB213" t="s">
         <v>1330</v>
       </c>
-      <c r="AE213" t="s">
+      <c r="AF213" t="s">
         <v>1232</v>
       </c>
     </row>
-    <row r="214" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A214" t="s">
         <v>951</v>
       </c>
@@ -13409,7 +13416,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="215" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A215" t="s">
         <v>952</v>
       </c>
@@ -13447,7 +13454,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="216" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A216" t="s">
         <v>953</v>
       </c>
@@ -13494,7 +13501,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="217" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A217" t="s">
         <v>1078</v>
       </c>
@@ -13541,7 +13548,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="218" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A218" t="s">
         <v>1081</v>
       </c>
@@ -13588,7 +13595,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="219" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A219" t="s">
         <v>1083</v>
       </c>
@@ -13635,7 +13642,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="220" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A220" t="s">
         <v>1085</v>
       </c>
@@ -13682,7 +13689,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="221" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A221" t="s">
         <v>1176</v>
       </c>
@@ -13723,7 +13730,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="222" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A222" t="s">
         <v>954</v>
       </c>
@@ -13764,7 +13771,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="223" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A223" t="s">
         <v>955</v>
       </c>
@@ -13802,7 +13809,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="224" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A224" t="s">
         <v>956</v>
       </c>
@@ -13846,7 +13853,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="225" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A225" t="s">
         <v>957</v>
       </c>
@@ -13890,7 +13897,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="226" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A226" t="s">
         <v>958</v>
       </c>
@@ -13928,7 +13935,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="227" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A227" t="s">
         <v>959</v>
       </c>
@@ -13972,7 +13979,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="228" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A228" t="s">
         <v>960</v>
       </c>
@@ -14013,7 +14020,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="229" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A229" t="s">
         <v>1088</v>
       </c>
@@ -14051,7 +14058,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="230" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A230" t="s">
         <v>1089</v>
       </c>
@@ -14104,7 +14111,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="231" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A231" t="s">
         <v>961</v>
       </c>
@@ -14147,11 +14154,11 @@
       <c r="AB231" t="s">
         <v>1330</v>
       </c>
-      <c r="AE231" t="s">
+      <c r="AF231" t="s">
         <v>1232</v>
       </c>
     </row>
-    <row r="232" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A232" t="s">
         <v>962</v>
       </c>
@@ -14195,7 +14202,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="233" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A233" t="s">
         <v>963</v>
       </c>
@@ -14239,7 +14246,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="234" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A234" t="s">
         <v>964</v>
       </c>
@@ -14277,7 +14284,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="235" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A235" t="s">
         <v>965</v>
       </c>
@@ -14315,7 +14322,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="236" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A236" t="s">
         <v>966</v>
       </c>
@@ -14353,7 +14360,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="237" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A237" t="s">
         <v>967</v>
       </c>
@@ -14397,7 +14404,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="238" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A238" t="s">
         <v>968</v>
       </c>
@@ -14444,7 +14451,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="239" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A239" t="s">
         <v>969</v>
       </c>
@@ -14488,7 +14495,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="240" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A240" t="s">
         <v>970</v>
       </c>
@@ -15841,7 +15848,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="273" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="273" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A273" t="s">
         <v>1212</v>
       </c>
@@ -15885,7 +15892,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="274" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="274" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A274" t="s">
         <v>995</v>
       </c>
@@ -15932,7 +15939,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="275" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="275" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A275" t="s">
         <v>996</v>
       </c>
@@ -15979,7 +15986,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="276" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="276" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A276" t="s">
         <v>997</v>
       </c>
@@ -16017,7 +16024,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="277" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="277" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A277" t="s">
         <v>998</v>
       </c>
@@ -16055,7 +16062,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="278" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="278" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A278" t="s">
         <v>999</v>
       </c>
@@ -16096,7 +16103,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="279" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="279" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A279" t="s">
         <v>1000</v>
       </c>
@@ -16134,7 +16141,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="280" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="280" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A280" t="s">
         <v>1018</v>
       </c>
@@ -16172,7 +16179,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="281" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="281" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A281" t="s">
         <v>1019</v>
       </c>
@@ -16216,7 +16223,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="282" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="282" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A282" t="s">
         <v>1020</v>
       </c>
@@ -16260,7 +16267,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="283" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="283" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A283" t="s">
         <v>1021</v>
       </c>
@@ -16304,7 +16311,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="284" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="284" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A284" t="s">
         <v>1001</v>
       </c>
@@ -16347,11 +16354,11 @@
       <c r="AB284" t="s">
         <v>1339</v>
       </c>
-      <c r="AE284" t="s">
+      <c r="AF284" t="s">
         <v>1231</v>
       </c>
     </row>
-    <row r="285" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="285" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A285" t="s">
         <v>1002</v>
       </c>
@@ -16392,7 +16399,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="286" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="286" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A286" t="s">
         <v>1227</v>
       </c>
@@ -16441,11 +16448,11 @@
       <c r="AB286" t="s">
         <v>1339</v>
       </c>
-      <c r="AE286" t="s">
+      <c r="AF286" t="s">
         <v>1225</v>
       </c>
     </row>
-    <row r="287" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="287" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A287" t="s">
         <v>1112</v>
       </c>
@@ -16489,7 +16496,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="288" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="288" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A288" t="s">
         <v>1262</v>
       </c>
@@ -16530,7 +16537,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="289" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="289" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A289" t="s">
         <v>1261</v>
       </c>
@@ -16571,7 +16578,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="290" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="290" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A290" t="s">
         <v>1217</v>
       </c>
@@ -16612,7 +16619,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="291" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="291" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A291" t="s">
         <v>1204</v>
       </c>
@@ -16653,7 +16660,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="292" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="292" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A292" t="s">
         <v>1165</v>
       </c>
@@ -16694,7 +16701,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="293" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="293" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A293" t="s">
         <v>1162</v>
       </c>
@@ -16732,7 +16739,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="294" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="294" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A294" t="s">
         <v>1233</v>
       </c>
@@ -16779,7 +16786,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="295" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="295" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A295" t="s">
         <v>1159</v>
       </c>
@@ -16814,7 +16821,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="296" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="296" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A296" t="s">
         <v>1003</v>
       </c>
@@ -16861,7 +16868,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="297" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="297" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A297" t="s">
         <v>1004</v>
       </c>
@@ -16902,7 +16909,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="298" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="298" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A298" t="s">
         <v>1168</v>
       </c>
@@ -16937,7 +16944,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="299" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="299" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A299" t="s">
         <v>1222</v>
       </c>
@@ -16984,7 +16991,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="300" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="300" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A300" t="s">
         <v>1223</v>
       </c>
@@ -17040,7 +17047,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="301" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="301" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A301" t="s">
         <v>1254</v>
       </c>
@@ -17096,7 +17103,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="302" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="302" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A302" t="s">
         <v>1121</v>
       </c>
@@ -17142,11 +17149,11 @@
       <c r="AB302" t="s">
         <v>1339</v>
       </c>
-      <c r="AE302" t="s">
+      <c r="AF302" t="s">
         <v>1228</v>
       </c>
     </row>
-    <row r="303" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="303" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A303" t="s">
         <v>1005</v>
       </c>
@@ -17181,7 +17188,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="304" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="304" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A304" t="s">
         <v>1265</v>
       </c>
@@ -18063,7 +18070,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AE283">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF283">
     <sortCondition ref="A2:A283"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>